<commit_message>
Fixed Issue with Title
</commit_message>
<xml_diff>
--- a/Results Summary PC.xlsx
+++ b/Results Summary PC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajayv\Documents\projects\UNI\22WSD530-Programming-Multi-many-core-Systems-Coursework-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D072CA5-8522-487A-A916-1BDD5C810C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC4BE92-9DF5-4A42-A05F-FD1760DB22C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -358,22 +358,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>152399</xdr:colOff>
+      <xdr:colOff>193674</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>268940</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>581026</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0427848C-3A29-A382-E92A-2F82981D1A8B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DC10A44-7BD8-A6A2-FC52-CBB100913141}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -395,8 +395,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8629649" y="1333500"/>
-          <a:ext cx="9127191" cy="5172075"/>
+          <a:off x="8670924" y="1343025"/>
+          <a:ext cx="10007602" cy="5629276"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -708,7 +708,7 @@
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated NN PC Results
</commit_message>
<xml_diff>
--- a/Results Summary PC.xlsx
+++ b/Results Summary PC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajayv\Documents\projects\UNI\22WSD530-Programming-Multi-many-core-Systems-Coursework-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC4BE92-9DF5-4A42-A05F-FD1760DB22C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C47CD62-EE57-405C-8D48-F04D654D8E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -358,22 +358,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>193674</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>182762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>581026</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
+      <xdr:rowOff>66676</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DC10A44-7BD8-A6A2-FC52-CBB100913141}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76EC5492-9A37-23F2-F0C1-10C96EF4EA57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -395,8 +395,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8670924" y="1343025"/>
-          <a:ext cx="10007602" cy="5629276"/>
+          <a:off x="8753475" y="1325762"/>
+          <a:ext cx="9953625" cy="5598914"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -708,7 +708,7 @@
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,13 +790,13 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
-        <v>17951700</v>
+        <v>12792500</v>
       </c>
       <c r="B3" s="14">
-        <v>16772800</v>
+        <v>14959900</v>
       </c>
       <c r="C3" s="15">
-        <v>119897800</v>
+        <v>121792400</v>
       </c>
       <c r="D3" s="13">
         <v>65385400</v>
@@ -824,34 +824,34 @@
       </c>
       <c r="N3" s="1">
         <f>SUM(A$3:A$102)/100</f>
-        <v>15429106</v>
+        <v>16628602</v>
       </c>
       <c r="O3" s="2">
         <f>SUM(B$3:B$102)/100</f>
-        <v>17730096</v>
+        <v>16366105</v>
       </c>
       <c r="P3" s="3">
         <f>SUM(C$3:C$102)/100</f>
-        <v>126218109</v>
+        <v>124924356</v>
       </c>
       <c r="Q3" s="1">
         <f>N3/O3</f>
-        <v>0.87022123286867703</v>
+        <v>1.016039063662368</v>
       </c>
       <c r="R3" s="3">
         <f>N3/P3</f>
-        <v>0.12224161906909888</v>
+        <v>0.13310936739990079</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
-        <v>13939500</v>
+        <v>16355100</v>
       </c>
       <c r="B4" s="17">
-        <v>18613800</v>
+        <v>13576200</v>
       </c>
       <c r="C4" s="18">
-        <v>129801700</v>
+        <v>122141700</v>
       </c>
       <c r="D4" s="16">
         <v>42286800</v>
@@ -900,13 +900,13 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
-        <v>13961900</v>
+        <v>14960900</v>
       </c>
       <c r="B5" s="17">
-        <v>17952100</v>
+        <v>16957100</v>
       </c>
       <c r="C5" s="18">
-        <v>126859600</v>
+        <v>124104300</v>
       </c>
       <c r="D5" s="16">
         <v>97599700</v>
@@ -953,13 +953,13 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
-        <v>19719800</v>
+        <v>23636500</v>
       </c>
       <c r="B6" s="17">
-        <v>30757100</v>
+        <v>17485600</v>
       </c>
       <c r="C6" s="18">
-        <v>122838800</v>
+        <v>130058400</v>
       </c>
       <c r="D6" s="16">
         <v>45716500</v>
@@ -1006,13 +1006,13 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
-        <v>15529600</v>
+        <v>15505200</v>
       </c>
       <c r="B7" s="17">
-        <v>19214100</v>
+        <v>24931600</v>
       </c>
       <c r="C7" s="18">
-        <v>124992700</v>
+        <v>129767300</v>
       </c>
       <c r="D7" s="16">
         <v>70889800</v>
@@ -1038,13 +1038,13 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
-        <v>14305700</v>
+        <v>14894200</v>
       </c>
       <c r="B8" s="17">
-        <v>18950100</v>
+        <v>14783000</v>
       </c>
       <c r="C8" s="18">
-        <v>131948200</v>
+        <v>123804300</v>
       </c>
       <c r="D8" s="16">
         <v>67141900</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
-        <v>13477500</v>
+        <v>13964700</v>
       </c>
       <c r="B9" s="17">
-        <v>15957100</v>
+        <v>15985400</v>
       </c>
       <c r="C9" s="18">
-        <v>124859100</v>
+        <v>139226600</v>
       </c>
       <c r="D9" s="16">
         <v>60474900</v>
@@ -1102,13 +1102,13 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
-        <v>12748600</v>
+        <v>15779900</v>
       </c>
       <c r="B10" s="17">
-        <v>15959100</v>
+        <v>15495200</v>
       </c>
       <c r="C10" s="18">
-        <v>123769200</v>
+        <v>131657300</v>
       </c>
       <c r="D10" s="16">
         <v>41308200</v>
@@ -1134,13 +1134,13 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
-        <v>15512700</v>
+        <v>37892700</v>
       </c>
       <c r="B11" s="17">
-        <v>19398700</v>
+        <v>23936900</v>
       </c>
       <c r="C11" s="18">
-        <v>120893100</v>
+        <v>126244200</v>
       </c>
       <c r="D11" s="16">
         <v>50724900</v>
@@ -1166,13 +1166,13 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
-        <v>15481300</v>
+        <v>14960300</v>
       </c>
       <c r="B12" s="17">
-        <v>15639400</v>
+        <v>16950600</v>
       </c>
       <c r="C12" s="18">
-        <v>117481200</v>
+        <v>124706300</v>
       </c>
       <c r="D12" s="16">
         <v>46803300</v>
@@ -1198,13 +1198,13 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
-        <v>14808400</v>
+        <v>16448900</v>
       </c>
       <c r="B13" s="17">
-        <v>15701400</v>
+        <v>12747200</v>
       </c>
       <c r="C13" s="18">
-        <v>125109700</v>
+        <v>122813100</v>
       </c>
       <c r="D13" s="16">
         <v>62673600</v>
@@ -1230,13 +1230,13 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
-        <v>16148000</v>
+        <v>16299100</v>
       </c>
       <c r="B14" s="17">
-        <v>40891400</v>
+        <v>19341800</v>
       </c>
       <c r="C14" s="18">
-        <v>124567700</v>
+        <v>126052100</v>
       </c>
       <c r="D14" s="16">
         <v>65463400</v>
@@ -1262,13 +1262,13 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
-        <v>16294400</v>
+        <v>35209200</v>
       </c>
       <c r="B15" s="17">
-        <v>14960400</v>
+        <v>16841900</v>
       </c>
       <c r="C15" s="18">
-        <v>125577300</v>
+        <v>129329600</v>
       </c>
       <c r="D15" s="16">
         <v>41513300</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
-        <v>19478000</v>
+        <v>14763000</v>
       </c>
       <c r="B16" s="17">
-        <v>17431400</v>
+        <v>16954800</v>
       </c>
       <c r="C16" s="18">
-        <v>119907900</v>
+        <v>126143400</v>
       </c>
       <c r="D16" s="16">
         <v>84401500</v>
@@ -1326,13 +1326,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
-        <v>15067000</v>
+        <v>16955600</v>
       </c>
       <c r="B17" s="17">
-        <v>17952300</v>
+        <v>15025200</v>
       </c>
       <c r="C17" s="18">
-        <v>137526000</v>
+        <v>118390700</v>
       </c>
       <c r="D17" s="16">
         <v>39769700</v>
@@ -1358,13 +1358,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
-        <v>18478700</v>
+        <v>12688700</v>
       </c>
       <c r="B18" s="17">
-        <v>16305700</v>
+        <v>13881600</v>
       </c>
       <c r="C18" s="18">
-        <v>114878700</v>
+        <v>122121800</v>
       </c>
       <c r="D18" s="16">
         <v>97018500</v>
@@ -1390,13 +1390,13 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
-        <v>15007900</v>
+        <v>14961500</v>
       </c>
       <c r="B19" s="17">
-        <v>41888500</v>
+        <v>17312900</v>
       </c>
       <c r="C19" s="18">
-        <v>115224200</v>
+        <v>117962500</v>
       </c>
       <c r="D19" s="16">
         <v>43088300</v>
@@ -1422,13 +1422,13 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
-        <v>21941500</v>
+        <v>23446500</v>
       </c>
       <c r="B20" s="17">
-        <v>13401800</v>
+        <v>13325700</v>
       </c>
       <c r="C20" s="18">
-        <v>124092300</v>
+        <v>121004300</v>
       </c>
       <c r="D20" s="16">
         <v>49565200</v>
@@ -1454,13 +1454,13 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
-        <v>15797100</v>
+        <v>15957800</v>
       </c>
       <c r="B21" s="17">
-        <v>20944600</v>
+        <v>22848500</v>
       </c>
       <c r="C21" s="18">
-        <v>124068500</v>
+        <v>134122300</v>
       </c>
       <c r="D21" s="16">
         <v>47099200</v>
@@ -1486,13 +1486,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
-        <v>14656900</v>
+        <v>13963100</v>
       </c>
       <c r="B22" s="17">
-        <v>19682600</v>
+        <v>13611800</v>
       </c>
       <c r="C22" s="18">
-        <v>116434300</v>
+        <v>124002100</v>
       </c>
       <c r="D22" s="16">
         <v>42656500</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
-        <v>13511400</v>
+        <v>16479100</v>
       </c>
       <c r="B23" s="17">
-        <v>16954700</v>
+        <v>19947200</v>
       </c>
       <c r="C23" s="18">
-        <v>145218000</v>
+        <v>123111000</v>
       </c>
       <c r="D23" s="16">
         <v>69927400</v>
@@ -1550,13 +1550,13 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
-        <v>29920000</v>
+        <v>16952800</v>
       </c>
       <c r="B24" s="17">
-        <v>15344800</v>
+        <v>15419000</v>
       </c>
       <c r="C24" s="18">
-        <v>123704900</v>
+        <v>125735200</v>
       </c>
       <c r="D24" s="16">
         <v>66148800</v>
@@ -1582,13 +1582,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
-        <v>17868500</v>
+        <v>15523100</v>
       </c>
       <c r="B25" s="17">
-        <v>13642800</v>
+        <v>15958900</v>
       </c>
       <c r="C25" s="18">
-        <v>129312600</v>
+        <v>123874100</v>
       </c>
       <c r="D25" s="16">
         <v>48179800</v>
@@ -1614,13 +1614,13 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
-        <v>14821900</v>
+        <v>14785600</v>
       </c>
       <c r="B26" s="17">
-        <v>13962500</v>
+        <v>15930400</v>
       </c>
       <c r="C26" s="18">
-        <v>140198200</v>
+        <v>122532500</v>
       </c>
       <c r="D26" s="16">
         <v>58580200</v>
@@ -1646,13 +1646,13 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
-        <v>12966300</v>
+        <v>15238400</v>
       </c>
       <c r="B27" s="17">
-        <v>18170000</v>
+        <v>15928000</v>
       </c>
       <c r="C27" s="18">
-        <v>127224200</v>
+        <v>127001800</v>
       </c>
       <c r="D27" s="16">
         <v>52244600</v>
@@ -1678,13 +1678,13 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
-        <v>17926900</v>
+        <v>16483100</v>
       </c>
       <c r="B28" s="17">
-        <v>20413300</v>
+        <v>14960600</v>
       </c>
       <c r="C28" s="18">
-        <v>119629700</v>
+        <v>118170200</v>
       </c>
       <c r="D28" s="16">
         <v>59274800</v>
@@ -1710,13 +1710,13 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
-        <v>19946900</v>
+        <v>18834800</v>
       </c>
       <c r="B29" s="17">
-        <v>14759000</v>
+        <v>15331800</v>
       </c>
       <c r="C29" s="18">
-        <v>129049500</v>
+        <v>132391900</v>
       </c>
       <c r="D29" s="16">
         <v>46482400</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
-        <v>12964900</v>
+        <v>15161700</v>
       </c>
       <c r="B30" s="17">
-        <v>15328800</v>
+        <v>13522400</v>
       </c>
       <c r="C30" s="18">
-        <v>137982700</v>
+        <v>119758100</v>
       </c>
       <c r="D30" s="16">
         <v>63174800</v>
@@ -1774,13 +1774,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
-        <v>14958800</v>
+        <v>16420300</v>
       </c>
       <c r="B31" s="17">
-        <v>15557100</v>
+        <v>14060500</v>
       </c>
       <c r="C31" s="18">
-        <v>122084200</v>
+        <v>123349400</v>
       </c>
       <c r="D31" s="16">
         <v>44964700</v>
@@ -1806,13 +1806,13 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
-        <v>13538300</v>
+        <v>15837900</v>
       </c>
       <c r="B32" s="17">
-        <v>15281800</v>
+        <v>27326800</v>
       </c>
       <c r="C32" s="18">
-        <v>125503400</v>
+        <v>123418900</v>
       </c>
       <c r="D32" s="16">
         <v>67703500</v>
@@ -1838,13 +1838,13 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
-        <v>15956500</v>
+        <v>13963200</v>
       </c>
       <c r="B33" s="17">
-        <v>14536100</v>
+        <v>14601900</v>
       </c>
       <c r="C33" s="18">
-        <v>147044100</v>
+        <v>123044200</v>
       </c>
       <c r="D33" s="16">
         <v>40642100</v>
@@ -1870,13 +1870,13 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
-        <v>17082200</v>
+        <v>13961400</v>
       </c>
       <c r="B34" s="17">
-        <v>15956900</v>
+        <v>13377300</v>
       </c>
       <c r="C34" s="18">
-        <v>126580600</v>
+        <v>116496200</v>
       </c>
       <c r="D34" s="16">
         <v>67929300</v>
@@ -1902,13 +1902,13 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
-        <v>13963200</v>
+        <v>13962500</v>
       </c>
       <c r="B35" s="17">
-        <v>17928100</v>
+        <v>15423000</v>
       </c>
       <c r="C35" s="18">
-        <v>121942000</v>
+        <v>122326700</v>
       </c>
       <c r="D35" s="16">
         <v>61834600</v>
@@ -1934,13 +1934,13 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="16">
-        <v>13962900</v>
+        <v>17831500</v>
       </c>
       <c r="B36" s="17">
-        <v>23935600</v>
+        <v>13454300</v>
       </c>
       <c r="C36" s="18">
-        <v>133994300</v>
+        <v>126282000</v>
       </c>
       <c r="D36" s="16">
         <v>43649000</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
-        <v>21723500</v>
+        <v>12965700</v>
       </c>
       <c r="B37" s="17">
-        <v>13960200</v>
+        <v>16738600</v>
       </c>
       <c r="C37" s="18">
-        <v>121346300</v>
+        <v>122872100</v>
       </c>
       <c r="D37" s="16">
         <v>54825500</v>
@@ -1998,13 +1998,13 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="16">
-        <v>12273800</v>
+        <v>13551900</v>
       </c>
       <c r="B38" s="17">
-        <v>16126800</v>
+        <v>13940100</v>
       </c>
       <c r="C38" s="18">
-        <v>122817600</v>
+        <v>121656600</v>
       </c>
       <c r="D38" s="16">
         <v>62943400</v>
@@ -2030,13 +2030,13 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="16">
-        <v>16331600</v>
+        <v>18950300</v>
       </c>
       <c r="B39" s="17">
-        <v>16210900</v>
+        <v>15382600</v>
       </c>
       <c r="C39" s="18">
-        <v>129571400</v>
+        <v>119203300</v>
       </c>
       <c r="D39" s="16">
         <v>66621000</v>
@@ -2062,13 +2062,13 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
-        <v>12426000</v>
+        <v>25934400</v>
       </c>
       <c r="B40" s="17">
-        <v>15723300</v>
+        <v>17549000</v>
       </c>
       <c r="C40" s="18">
-        <v>124856300</v>
+        <v>120772600</v>
       </c>
       <c r="D40" s="16">
         <v>58697700</v>
@@ -2094,13 +2094,13 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
-        <v>21860600</v>
+        <v>13963500</v>
       </c>
       <c r="B41" s="17">
-        <v>24934200</v>
+        <v>14572700</v>
       </c>
       <c r="C41" s="18">
-        <v>124589100</v>
+        <v>128303400</v>
       </c>
       <c r="D41" s="16">
         <v>43172000</v>
@@ -2126,13 +2126,13 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="16">
-        <v>13543800</v>
+        <v>14285400</v>
       </c>
       <c r="B42" s="17">
-        <v>13107600</v>
+        <v>14960500</v>
       </c>
       <c r="C42" s="18">
-        <v>141944500</v>
+        <v>129951600</v>
       </c>
       <c r="D42" s="16">
         <v>74345200</v>
@@ -2158,13 +2158,13 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="16">
-        <v>13547200</v>
+        <v>15958000</v>
       </c>
       <c r="B43" s="17">
-        <v>16313800</v>
+        <v>14476800</v>
       </c>
       <c r="C43" s="18">
-        <v>126395300</v>
+        <v>129832200</v>
       </c>
       <c r="D43" s="16">
         <v>43190300</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="16">
-        <v>14960600</v>
+        <v>13610500</v>
       </c>
       <c r="B44" s="17">
-        <v>14969800</v>
+        <v>15292900</v>
       </c>
       <c r="C44" s="18">
-        <v>127235200</v>
+        <v>127714700</v>
       </c>
       <c r="D44" s="16">
         <v>79555900</v>
@@ -2222,13 +2222,13 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="16">
-        <v>14347400</v>
+        <v>20945200</v>
       </c>
       <c r="B45" s="17">
-        <v>15958300</v>
+        <v>22939100</v>
       </c>
       <c r="C45" s="18">
-        <v>138677800</v>
+        <v>123029500</v>
       </c>
       <c r="D45" s="16">
         <v>42134700</v>
@@ -2254,13 +2254,13 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
-        <v>17948000</v>
+        <v>14757100</v>
       </c>
       <c r="B46" s="17">
-        <v>23456600</v>
+        <v>12965900</v>
       </c>
       <c r="C46" s="18">
-        <v>125216500</v>
+        <v>122753800</v>
       </c>
       <c r="D46" s="16">
         <v>54387300</v>
@@ -2286,13 +2286,13 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
-        <v>12705300</v>
+        <v>15770900</v>
       </c>
       <c r="B47" s="17">
-        <v>13480500</v>
+        <v>15748300</v>
       </c>
       <c r="C47" s="18">
-        <v>116599800</v>
+        <v>124660200</v>
       </c>
       <c r="D47" s="16">
         <v>42288400</v>
@@ -2318,13 +2318,13 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="16">
-        <v>13500800</v>
+        <v>18951300</v>
       </c>
       <c r="B48" s="17">
-        <v>12790300</v>
+        <v>15918400</v>
       </c>
       <c r="C48" s="18">
-        <v>135161800</v>
+        <v>127973400</v>
       </c>
       <c r="D48" s="16">
         <v>59412100</v>
@@ -2350,13 +2350,13 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="16">
-        <v>14115100</v>
+        <v>14320000</v>
       </c>
       <c r="B49" s="17">
-        <v>13964100</v>
+        <v>14936100</v>
       </c>
       <c r="C49" s="18">
-        <v>119939900</v>
+        <v>121810200</v>
       </c>
       <c r="D49" s="16">
         <v>46668900</v>
@@ -2382,13 +2382,13 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
-        <v>13797600</v>
+        <v>22279900</v>
       </c>
       <c r="B50" s="17">
-        <v>19852700</v>
+        <v>14962000</v>
       </c>
       <c r="C50" s="18">
-        <v>120023300</v>
+        <v>134156000</v>
       </c>
       <c r="D50" s="16">
         <v>45877100</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
-        <v>16573300</v>
+        <v>12966800</v>
       </c>
       <c r="B51" s="17">
-        <v>14584100</v>
+        <v>15757100</v>
       </c>
       <c r="C51" s="18">
-        <v>134917100</v>
+        <v>114030300</v>
       </c>
       <c r="D51" s="16">
         <v>46341300</v>
@@ -2446,13 +2446,13 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
-        <v>14286700</v>
+        <v>16047900</v>
       </c>
       <c r="B52" s="17">
-        <v>15957900</v>
+        <v>15957300</v>
       </c>
       <c r="C52" s="18">
-        <v>123686800</v>
+        <v>117719900</v>
       </c>
       <c r="D52" s="16">
         <v>83265800</v>
@@ -2478,13 +2478,13 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
-        <v>14402300</v>
+        <v>16102400</v>
       </c>
       <c r="B53" s="17">
-        <v>14960300</v>
+        <v>17760700</v>
       </c>
       <c r="C53" s="18">
-        <v>122167200</v>
+        <v>127266200</v>
       </c>
       <c r="D53" s="16">
         <v>38974100</v>
@@ -2510,13 +2510,13 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
-        <v>13552000</v>
+        <v>13366400</v>
       </c>
       <c r="B54" s="17">
-        <v>15957700</v>
+        <v>14957700</v>
       </c>
       <c r="C54" s="18">
-        <v>130550700</v>
+        <v>124349700</v>
       </c>
       <c r="D54" s="16">
         <v>62008400</v>
@@ -2542,13 +2542,13 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="16">
-        <v>15952600</v>
+        <v>26495700</v>
       </c>
       <c r="B55" s="17">
-        <v>15488000</v>
+        <v>15734300</v>
       </c>
       <c r="C55" s="18">
-        <v>127229900</v>
+        <v>119816200</v>
       </c>
       <c r="D55" s="16">
         <v>61975500</v>
@@ -2574,13 +2574,13 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="16">
-        <v>12900900</v>
+        <v>15481400</v>
       </c>
       <c r="B56" s="17">
-        <v>15408800</v>
+        <v>15346200</v>
       </c>
       <c r="C56" s="18">
-        <v>125281600</v>
+        <v>135660500</v>
       </c>
       <c r="D56" s="16">
         <v>42744700</v>
@@ -2606,13 +2606,13 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="16">
-        <v>13931800</v>
+        <v>13805500</v>
       </c>
       <c r="B57" s="17">
-        <v>19327200</v>
+        <v>18949900</v>
       </c>
       <c r="C57" s="18">
-        <v>131706900</v>
+        <v>139436200</v>
       </c>
       <c r="D57" s="16">
         <v>80928700</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="16">
-        <v>19947100</v>
+        <v>13037600</v>
       </c>
       <c r="B58" s="17">
-        <v>23485200</v>
+        <v>15655000</v>
       </c>
       <c r="C58" s="18">
-        <v>122915100</v>
+        <v>126853400</v>
       </c>
       <c r="D58" s="16">
         <v>44573500</v>
@@ -2670,13 +2670,13 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="16">
-        <v>20327700</v>
+        <v>13775800</v>
       </c>
       <c r="B59" s="17">
-        <v>14960300</v>
+        <v>13963600</v>
       </c>
       <c r="C59" s="18">
-        <v>136301500</v>
+        <v>126521100</v>
       </c>
       <c r="D59" s="16">
         <v>48988800</v>
@@ -2702,13 +2702,13 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="16">
-        <v>13340600</v>
+        <v>17952900</v>
       </c>
       <c r="B60" s="17">
-        <v>13509500</v>
+        <v>13936100</v>
       </c>
       <c r="C60" s="18">
-        <v>127659800</v>
+        <v>125196000</v>
       </c>
       <c r="D60" s="16">
         <v>74022000</v>
@@ -2734,13 +2734,13 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="16">
-        <v>13432900</v>
+        <v>14960600</v>
       </c>
       <c r="B61" s="17">
-        <v>16955200</v>
+        <v>13938300</v>
       </c>
       <c r="C61" s="18">
-        <v>120631000</v>
+        <v>115234400</v>
       </c>
       <c r="D61" s="16">
         <v>40555100</v>
@@ -2766,13 +2766,13 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="16">
-        <v>12965900</v>
+        <v>13536500</v>
       </c>
       <c r="B62" s="17">
-        <v>14097300</v>
+        <v>27630200</v>
       </c>
       <c r="C62" s="18">
-        <v>123480400</v>
+        <v>123369100</v>
       </c>
       <c r="D62" s="16">
         <v>66523200</v>
@@ -2798,13 +2798,13 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="16">
-        <v>13733300</v>
+        <v>15958800</v>
       </c>
       <c r="B63" s="17">
-        <v>16718000</v>
+        <v>14627500</v>
       </c>
       <c r="C63" s="18">
-        <v>126706900</v>
+        <v>127811100</v>
       </c>
       <c r="D63" s="16">
         <v>61288100</v>
@@ -2830,13 +2830,13 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="16">
-        <v>12965200</v>
+        <v>15840000</v>
       </c>
       <c r="B64" s="17">
-        <v>13785900</v>
+        <v>14580200</v>
       </c>
       <c r="C64" s="18">
-        <v>124194400</v>
+        <v>118295400</v>
       </c>
       <c r="D64" s="16">
         <v>54948000</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="16">
-        <v>14295200</v>
+        <v>12965600</v>
       </c>
       <c r="B65" s="17">
-        <v>18950000</v>
+        <v>14937700</v>
       </c>
       <c r="C65" s="18">
-        <v>116918400</v>
+        <v>134443400</v>
       </c>
       <c r="D65" s="16">
         <v>41269500</v>
@@ -2894,13 +2894,13 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="16">
-        <v>18106200</v>
+        <v>14482000</v>
       </c>
       <c r="B66" s="17">
-        <v>38897000</v>
+        <v>13964300</v>
       </c>
       <c r="C66" s="18">
-        <v>131113100</v>
+        <v>117438400</v>
       </c>
       <c r="D66" s="16">
         <v>76985700</v>
@@ -2926,13 +2926,13 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="16">
-        <v>18949600</v>
+        <v>19947000</v>
       </c>
       <c r="B67" s="17">
-        <v>14584700</v>
+        <v>34902600</v>
       </c>
       <c r="C67" s="18">
-        <v>138065400</v>
+        <v>131834100</v>
       </c>
       <c r="D67" s="16">
         <v>42838800</v>
@@ -2958,13 +2958,13 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="16">
-        <v>12965500</v>
+        <v>13963000</v>
       </c>
       <c r="B68" s="17">
-        <v>20949500</v>
+        <v>13861500</v>
       </c>
       <c r="C68" s="18">
-        <v>119679300</v>
+        <v>153868000</v>
       </c>
       <c r="D68" s="16">
         <v>40212700</v>
@@ -2990,13 +2990,13 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="16">
-        <v>14365800</v>
+        <v>12966200</v>
       </c>
       <c r="B69" s="17">
-        <v>14860500</v>
+        <v>13938300</v>
       </c>
       <c r="C69" s="18">
-        <v>129036800</v>
+        <v>130495900</v>
       </c>
       <c r="D69" s="16">
         <v>84575500</v>
@@ -3022,13 +3022,13 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="16">
-        <v>14064800</v>
+        <v>14807400</v>
       </c>
       <c r="B70" s="17">
-        <v>14958500</v>
+        <v>13520700</v>
       </c>
       <c r="C70" s="18">
-        <v>132773700</v>
+        <v>121963600</v>
       </c>
       <c r="D70" s="16">
         <v>41217700</v>
@@ -3054,13 +3054,13 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="16">
-        <v>15957700</v>
+        <v>15958800</v>
       </c>
       <c r="B71" s="17">
-        <v>17498900</v>
+        <v>15774700</v>
       </c>
       <c r="C71" s="18">
-        <v>117194500</v>
+        <v>128936400</v>
       </c>
       <c r="D71" s="16">
         <v>46876400</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="16">
-        <v>14185800</v>
+        <v>14960200</v>
       </c>
       <c r="B72" s="17">
-        <v>14789100</v>
+        <v>13772800</v>
       </c>
       <c r="C72" s="18">
-        <v>128318500</v>
+        <v>117110800</v>
       </c>
       <c r="D72" s="16">
         <v>70022700</v>
@@ -3118,13 +3118,13 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="16">
-        <v>13960400</v>
+        <v>13690400</v>
       </c>
       <c r="B73" s="17">
-        <v>14961200</v>
+        <v>13405700</v>
       </c>
       <c r="C73" s="18">
-        <v>123252800</v>
+        <v>118399700</v>
       </c>
       <c r="D73" s="16">
         <v>43883100</v>
@@ -3150,13 +3150,13 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="16">
-        <v>12965600</v>
+        <v>13799100</v>
       </c>
       <c r="B74" s="17">
-        <v>18311100</v>
+        <v>14961700</v>
       </c>
       <c r="C74" s="18">
-        <v>126018800</v>
+        <v>138723900</v>
       </c>
       <c r="D74" s="16">
         <v>45878200</v>
@@ -3182,13 +3182,13 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="16">
-        <v>21491400</v>
+        <v>15654900</v>
       </c>
       <c r="B75" s="17">
-        <v>14480300</v>
+        <v>21083900</v>
       </c>
       <c r="C75" s="18">
-        <v>118542200</v>
+        <v>129955800</v>
       </c>
       <c r="D75" s="16">
         <v>85630300</v>
@@ -3214,13 +3214,13 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="16">
-        <v>13753100</v>
+        <v>34718000</v>
       </c>
       <c r="B76" s="17">
-        <v>15957700</v>
+        <v>15466700</v>
       </c>
       <c r="C76" s="18">
-        <v>127382000</v>
+        <v>118997700</v>
       </c>
       <c r="D76" s="16">
         <v>41284400</v>
@@ -3246,13 +3246,13 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="16">
-        <v>13958600</v>
+        <v>14408300</v>
       </c>
       <c r="B77" s="17">
-        <v>20944800</v>
+        <v>14806600</v>
       </c>
       <c r="C77" s="18">
-        <v>123530500</v>
+        <v>126556800</v>
       </c>
       <c r="D77" s="16">
         <v>49160200</v>
@@ -3278,13 +3278,13 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="16">
-        <v>14959800</v>
+        <v>12966000</v>
       </c>
       <c r="B78" s="17">
-        <v>35433700</v>
+        <v>13961900</v>
       </c>
       <c r="C78" s="18">
-        <v>122894700</v>
+        <v>120249600</v>
       </c>
       <c r="D78" s="16">
         <v>56795400</v>
@@ -3310,13 +3310,13 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="16">
-        <v>14283900</v>
+        <v>12680300</v>
       </c>
       <c r="B79" s="17">
-        <v>16328600</v>
+        <v>16293800</v>
       </c>
       <c r="C79" s="18">
-        <v>138959100</v>
+        <v>124557100</v>
       </c>
       <c r="D79" s="16">
         <v>42349700</v>
@@ -3342,13 +3342,13 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="16">
-        <v>19942400</v>
+        <v>14484500</v>
       </c>
       <c r="B80" s="17">
-        <v>15957600</v>
+        <v>15422100</v>
       </c>
       <c r="C80" s="18">
-        <v>128081700</v>
+        <v>136476700</v>
       </c>
       <c r="D80" s="16">
         <v>67168200</v>
@@ -3374,13 +3374,13 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="16">
-        <v>15783200</v>
+        <v>14959600</v>
       </c>
       <c r="B81" s="17">
-        <v>16202600</v>
+        <v>13958300</v>
       </c>
       <c r="C81" s="18">
-        <v>115976800</v>
+        <v>127340900</v>
       </c>
       <c r="D81" s="16">
         <v>59167900</v>
@@ -3406,13 +3406,13 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="16">
-        <v>13493800</v>
+        <v>13798900</v>
       </c>
       <c r="B82" s="17">
-        <v>29706400</v>
+        <v>16017400</v>
       </c>
       <c r="C82" s="18">
-        <v>117986400</v>
+        <v>121421700</v>
       </c>
       <c r="D82" s="16">
         <v>63112000</v>
@@ -3438,13 +3438,13 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="16">
-        <v>12671500</v>
+        <v>15610200</v>
       </c>
       <c r="B83" s="17">
-        <v>16182400</v>
+        <v>15957500</v>
       </c>
       <c r="C83" s="18">
-        <v>116858400</v>
+        <v>123823000</v>
       </c>
       <c r="D83" s="16">
         <v>37898900</v>
@@ -3470,13 +3470,13 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="16">
-        <v>13741700</v>
+        <v>16282100</v>
       </c>
       <c r="B84" s="17">
-        <v>15590800</v>
+        <v>16523700</v>
       </c>
       <c r="C84" s="18">
-        <v>138091400</v>
+        <v>115635000</v>
       </c>
       <c r="D84" s="16">
         <v>56822900</v>
@@ -3502,13 +3502,13 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="16">
-        <v>17344800</v>
+        <v>15623500</v>
       </c>
       <c r="B85" s="17">
-        <v>15888900</v>
+        <v>15504500</v>
       </c>
       <c r="C85" s="18">
-        <v>121084700</v>
+        <v>118110700</v>
       </c>
       <c r="D85" s="16">
         <v>57507500</v>
@@ -3534,13 +3534,13 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="16">
-        <v>13513200</v>
+        <v>12966300</v>
       </c>
       <c r="B86" s="17">
-        <v>14937900</v>
+        <v>15593600</v>
       </c>
       <c r="C86" s="18">
-        <v>134030900</v>
+        <v>126749300</v>
       </c>
       <c r="D86" s="16">
         <v>42888500</v>
@@ -3566,13 +3566,13 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="16">
-        <v>16800400</v>
+        <v>13797800</v>
       </c>
       <c r="B87" s="17">
-        <v>25931100</v>
+        <v>14961400</v>
       </c>
       <c r="C87" s="18">
-        <v>116487500</v>
+        <v>122078400</v>
       </c>
       <c r="D87" s="16">
         <v>68356800</v>
@@ -3598,13 +3598,13 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="16">
-        <v>19362700</v>
+        <v>16156400</v>
       </c>
       <c r="B88" s="17">
-        <v>14747300</v>
+        <v>14667800</v>
       </c>
       <c r="C88" s="18">
-        <v>117354900</v>
+        <v>128632000</v>
       </c>
       <c r="D88" s="16">
         <v>41980200</v>
@@ -3630,13 +3630,13 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="16">
-        <v>14809300</v>
+        <v>35528300</v>
       </c>
       <c r="B89" s="17">
-        <v>14961500</v>
+        <v>16954600</v>
       </c>
       <c r="C89" s="18">
-        <v>124912800</v>
+        <v>125746500</v>
       </c>
       <c r="D89" s="16">
         <v>54086900</v>
@@ -3662,13 +3662,13 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="16">
-        <v>14482600</v>
+        <v>13962400</v>
       </c>
       <c r="B90" s="17">
-        <v>17736100</v>
+        <v>13962800</v>
       </c>
       <c r="C90" s="18">
-        <v>119114200</v>
+        <v>121276300</v>
       </c>
       <c r="D90" s="16">
         <v>62730100</v>
@@ -3694,13 +3694,13 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="16">
-        <v>12517900</v>
+        <v>14836200</v>
       </c>
       <c r="B91" s="17">
-        <v>14570000</v>
+        <v>20944800</v>
       </c>
       <c r="C91" s="18">
-        <v>138042300</v>
+        <v>121591800</v>
       </c>
       <c r="D91" s="16">
         <v>42926000</v>
@@ -3726,13 +3726,13 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="16">
-        <v>13788800</v>
+        <v>17182300</v>
       </c>
       <c r="B92" s="17">
-        <v>14629300</v>
+        <v>14695300</v>
       </c>
       <c r="C92" s="18">
-        <v>123773700</v>
+        <v>132319900</v>
       </c>
       <c r="D92" s="16">
         <v>79012400</v>
@@ -3758,13 +3758,13 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="16">
-        <v>15826800</v>
+        <v>20661000</v>
       </c>
       <c r="B93" s="17">
-        <v>16836100</v>
+        <v>14659700</v>
       </c>
       <c r="C93" s="18">
-        <v>129220800</v>
+        <v>122708900</v>
       </c>
       <c r="D93" s="16">
         <v>41312800</v>
@@ -3790,13 +3790,13 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="16">
-        <v>14592700</v>
+        <v>13814900</v>
       </c>
       <c r="B94" s="17">
-        <v>12961900</v>
+        <v>18262000</v>
       </c>
       <c r="C94" s="18">
-        <v>122828100</v>
+        <v>122021400</v>
       </c>
       <c r="D94" s="16">
         <v>56968000</v>
@@ -3822,13 +3822,13 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="16">
-        <v>13970200</v>
+        <v>13611300</v>
       </c>
       <c r="B95" s="17">
-        <v>16666100</v>
+        <v>18276300</v>
       </c>
       <c r="C95" s="18">
-        <v>117786500</v>
+        <v>125043400</v>
       </c>
       <c r="D95" s="16">
         <v>62083200</v>
@@ -3854,13 +3854,13 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="16">
-        <v>12315200</v>
+        <v>13793000</v>
       </c>
       <c r="B96" s="17">
-        <v>14959000</v>
+        <v>20840800</v>
       </c>
       <c r="C96" s="18">
-        <v>117977100</v>
+        <v>120249300</v>
       </c>
       <c r="D96" s="16">
         <v>48675300</v>
@@ -3886,13 +3886,13 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="16">
-        <v>12747400</v>
+        <v>14511100</v>
       </c>
       <c r="B97" s="17">
-        <v>15957600</v>
+        <v>14767500</v>
       </c>
       <c r="C97" s="18">
-        <v>147144200</v>
+        <v>119998400</v>
       </c>
       <c r="D97" s="16">
         <v>41774000</v>
@@ -3918,13 +3918,13 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="16">
-        <v>20282300</v>
+        <v>31861400</v>
       </c>
       <c r="B98" s="17">
-        <v>17132700</v>
+        <v>14522100</v>
       </c>
       <c r="C98" s="18">
-        <v>124770900</v>
+        <v>126853000</v>
       </c>
       <c r="D98" s="16">
         <v>57118900</v>
@@ -3950,13 +3950,13 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="16">
-        <v>13963000</v>
+        <v>13778800</v>
       </c>
       <c r="B99" s="17">
-        <v>13962400</v>
+        <v>14744100</v>
       </c>
       <c r="C99" s="18">
-        <v>130856600</v>
+        <v>118551100</v>
       </c>
       <c r="D99" s="16">
         <v>57143600</v>
@@ -3982,13 +3982,13 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="16">
-        <v>13324800</v>
+        <v>15958200</v>
       </c>
       <c r="B100" s="17">
-        <v>17416500</v>
+        <v>22935200</v>
       </c>
       <c r="C100" s="18">
-        <v>125559600</v>
+        <v>115211700</v>
       </c>
       <c r="D100" s="16">
         <v>52751400</v>
@@ -4014,13 +4014,13 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="16">
-        <v>13387700</v>
+        <v>19309600</v>
       </c>
       <c r="B101" s="17">
-        <v>18016700</v>
+        <v>19881400</v>
       </c>
       <c r="C101" s="18">
-        <v>124263500</v>
+        <v>127934700</v>
       </c>
       <c r="D101" s="16">
         <v>50171800</v>
@@ -4046,13 +4046,13 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="19">
-        <v>14896300</v>
+        <v>13962000</v>
       </c>
       <c r="B102" s="20">
-        <v>13962700</v>
+        <v>16532600</v>
       </c>
       <c r="C102" s="21">
-        <v>123927600</v>
+        <v>119944300</v>
       </c>
       <c r="D102" s="19">
         <v>40015200</v>

</xml_diff>